<commit_message>
Update based on PGA
</commit_message>
<xml_diff>
--- a/data/Edison's Scores.xlsx
+++ b/data/Edison's Scores.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="571">
   <si>
     <t>Course</t>
   </si>
@@ -822,7 +822,7 @@
     <t>5,250,4,3,7,X</t>
   </si>
   <si>
-    <t>PGA Course</t>
+    <t>PGA Wanamaker</t>
   </si>
   <si>
     <t>4,177,3,2,5,Y</t>
@@ -1627,6 +1627,108 @@
   </si>
   <si>
     <t>5,375,2,2,4,Y</t>
+  </si>
+  <si>
+    <t>PGA Ryder - Front</t>
+  </si>
+  <si>
+    <t>4,232,2,2,4,X</t>
+  </si>
+  <si>
+    <t>4,226,2,3,5,Y</t>
+  </si>
+  <si>
+    <t>5,312,2,4,6,Y</t>
+  </si>
+  <si>
+    <t>3,109,1,2,3,Y</t>
+  </si>
+  <si>
+    <t>5,330,3,3,6,Y</t>
+  </si>
+  <si>
+    <t>3,120,2,2,4,Y</t>
+  </si>
+  <si>
+    <t>4,235,4,2,6,X</t>
+  </si>
+  <si>
+    <t>4,263,2,2,4,Y</t>
+  </si>
+  <si>
+    <t>PGA Ryder - Back</t>
+  </si>
+  <si>
+    <t>3,100,1,2,3,Y</t>
+  </si>
+  <si>
+    <t>4,240,2,3,5,Y</t>
+  </si>
+  <si>
+    <t>3,112,1,2,3,Y</t>
+  </si>
+  <si>
+    <t>5,386, 4,2,6,Y</t>
+  </si>
+  <si>
+    <t>4,264,3,1,4,Y</t>
+  </si>
+  <si>
+    <t>5,351,5,1,6,Y</t>
+  </si>
+  <si>
+    <t>3,105,2,2,4,X</t>
+  </si>
+  <si>
+    <t>5,342,4,2,6,X</t>
+  </si>
+  <si>
+    <t>4,236,2,2,4,Y</t>
+  </si>
+  <si>
+    <t>4,232,5,2,7,X</t>
+  </si>
+  <si>
+    <t>4,226,3,3,6,X</t>
+  </si>
+  <si>
+    <t>5,312,3,2,5,X</t>
+  </si>
+  <si>
+    <t>3,109,1,3,4,Y</t>
+  </si>
+  <si>
+    <t>3,120,1,2,3,X</t>
+  </si>
+  <si>
+    <t>4,235,2,2,4,Y</t>
+  </si>
+  <si>
+    <t>4,265,2,2,4,Y</t>
+  </si>
+  <si>
+    <t>4,100,5,2,7,X</t>
+  </si>
+  <si>
+    <t>4,240,2,3,5,X</t>
+  </si>
+  <si>
+    <t>3,112,2,2,4,Y</t>
+  </si>
+  <si>
+    <t>5,386,4,2,6,Y</t>
+  </si>
+  <si>
+    <t>4,244,3,3,6,Y</t>
+  </si>
+  <si>
+    <t>5,351,3,2,5,X</t>
+  </si>
+  <si>
+    <t>3,105,1,2,3,Y</t>
+  </si>
+  <si>
+    <t>4,236,3,2,5,X</t>
   </si>
 </sst>
 </file>
@@ -4184,7 +4286,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="2" t="s">
         <v>79</v>
       </c>
@@ -4225,7 +4327,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="2" t="s">
         <v>58</v>
       </c>
@@ -4266,7 +4368,7 @@
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="2" t="s">
         <v>101</v>
       </c>
@@ -4307,7 +4409,7 @@
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="2" t="s">
         <v>88</v>
       </c>
@@ -4348,7 +4450,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="2" t="s">
         <v>101</v>
       </c>
@@ -4389,7 +4491,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="2" t="s">
         <v>69</v>
       </c>
@@ -4430,7 +4532,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="2" t="s">
         <v>79</v>
       </c>
@@ -4471,7 +4573,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
       <c r="A60" s="2" t="s">
         <v>505</v>
       </c>
@@ -4512,7 +4614,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="2" t="s">
         <v>515</v>
       </c>
@@ -4553,11 +4655,11 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
       <c r="A62" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B62" s="4" t="s">
         <v>481</v>
       </c>
       <c r="C62" s="3">
@@ -4594,11 +4696,11 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
       <c r="A63" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="4" t="s">
         <v>481</v>
       </c>
       <c r="C63" s="3">
@@ -4635,67 +4737,171 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="20.25">
-      <c r="A64" s="2"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
-      <c r="M64" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="20.25">
-      <c r="A65" s="2"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
-      <c r="L65" s="2"/>
-      <c r="M65" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="20.25">
-      <c r="A66" s="2"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
-      <c r="K66" s="2"/>
-      <c r="L66" s="2"/>
-      <c r="M66" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="20.25">
-      <c r="A67" s="2"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
-      <c r="L67" s="2"/>
-      <c r="M67" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
+      <c r="A64" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="C64" s="3">
+        <v>45941</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="M64" s="10">
+        <v>42</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
+      <c r="A65" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="C65" s="3">
+        <v>45941</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="M65" s="10">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
+      <c r="A66" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="C66" s="3">
+        <v>45942</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="M66" s="10">
+        <v>44</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
+      <c r="A67" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="C67" s="3">
+        <v>45942</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="M67" s="10">
+        <v>46</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
       <c r="A68" s="2"/>
       <c r="B68" s="10"/>
       <c r="C68" s="3"/>
@@ -4710,7 +4916,7 @@
       <c r="L68" s="2"/>
       <c r="M68" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
       <c r="A69" s="2"/>
       <c r="B69" s="10"/>
       <c r="C69" s="3"/>

</xml_diff>